<commit_message>
Final bulk import: > separator, Excel input, duplicate detection, mixed categories
</commit_message>
<xml_diff>
--- a/templates/example_bulk_import1.xlsx
+++ b/templates/example_bulk_import1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\0_Sasa\events-tracker\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05D84574-33E3-4023-908F-FDEE80103ED3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC85571D-6BA8-425B-91C2-615D2A37F9BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40785" yWindow="375" windowWidth="15255" windowHeight="13290" xr2:uid="{FCD908A9-9BC7-4AC8-A3EF-A40EE0A34CC3}"/>
+    <workbookView xWindow="34590" yWindow="1305" windowWidth="17220" windowHeight="9510" xr2:uid="{FCD908A9-9BC7-4AC8-A3EF-A40EE0A34CC3}"/>
   </bookViews>
   <sheets>
     <sheet name="example_bulk_import" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
   <si>
     <t>Category</t>
   </si>
@@ -31,21 +31,12 @@
     <t>Comment</t>
   </si>
   <si>
-    <t>Health â†’ Sleep</t>
-  </si>
-  <si>
-    <t>Training â†’ Cardio â†’ Upper Body</t>
-  </si>
-  <si>
     <t>Total Sleep</t>
   </si>
   <si>
     <t>Sleep Quality</t>
   </si>
   <si>
-    <t>Health â†’ Daily Wellness</t>
-  </si>
-  <si>
     <t>Comment 1</t>
   </si>
   <si>
@@ -67,10 +58,10 @@
     <t>Comment 4</t>
   </si>
   <si>
-    <t>Comment 5</t>
-  </si>
-  <si>
-    <t>Comment 6</t>
+    <t>Health &gt; Sleep</t>
+  </si>
+  <si>
+    <t>Health &gt; Daily Wellness</t>
   </si>
 </sst>
 </file>
@@ -579,10 +570,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -958,10 +948,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D1F63E0-F7F5-4B2F-9B3D-018495760E64}">
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -982,19 +972,19 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
         <v>6</v>
       </c>
-      <c r="E1" t="s">
-        <v>9</v>
-      </c>
       <c r="F1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="G1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="H1" t="s">
         <v>2</v>
@@ -1002,7 +992,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="B2" s="1">
         <v>45974</v>
@@ -1014,15 +1004,15 @@
         <v>77</v>
       </c>
       <c r="H2" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="B3" s="1">
-        <v>45973</v>
+        <v>45971</v>
       </c>
       <c r="C3">
         <v>8</v>
@@ -1031,15 +1021,15 @@
         <v>22</v>
       </c>
       <c r="H3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="B4" s="1">
-        <v>45974</v>
+        <v>45972</v>
       </c>
       <c r="E4">
         <v>10001</v>
@@ -1051,15 +1041,15 @@
         <v>42</v>
       </c>
       <c r="H4" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="B5" s="1">
-        <v>45974</v>
+        <v>45970</v>
       </c>
       <c r="E5">
         <v>10001</v>
@@ -1071,31 +1061,7 @@
         <v>37</v>
       </c>
       <c r="H5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="1">
-        <v>45973</v>
-      </c>
-      <c r="E6" s="2"/>
-      <c r="H6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" s="1">
-        <v>45974</v>
-      </c>
-      <c r="E7" s="2"/>
-      <c r="H7" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>